<commit_message>
Daily sync 16/03, end of week 5
Updated progress on planning doc, added Tasks file as a kind of low level to do list and backlog tracker
</commit_message>
<xml_diff>
--- a/Planning_Internship_Thesis.xlsx
+++ b/Planning_Internship_Thesis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="8175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="10290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>Define the deployment Architecture</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>Prepare for the "tussentijdse evaluatie"</t>
-  </si>
-  <si>
-    <t>Presentations on 27th and 28th of March</t>
   </si>
   <si>
     <t>3.4.4</t>
@@ -260,6 +257,15 @@
   </si>
   <si>
     <t>Find a way to not get fucked by power outages or machine crashes</t>
+  </si>
+  <si>
+    <t>Presentation on 27/03 at 11:30 in room A118</t>
+  </si>
+  <si>
+    <t>Currently works for chrome</t>
+  </si>
+  <si>
+    <t>Idk, It should be fine? Might not be 100% bug free, so I'm putting it on finished, but not 100%</t>
   </si>
 </sst>
 </file>
@@ -692,7 +698,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,15 +794,15 @@
         <v>0.2</v>
       </c>
       <c r="I7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
         <v>74</v>
-      </c>
-      <c r="B8" t="s">
-        <v>75</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -840,7 +846,7 @@
         <v>10</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -848,7 +854,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="14">
         <v>1</v>
@@ -857,7 +863,7 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -908,7 +914,10 @@
         <v>25</v>
       </c>
       <c r="E17" s="14">
-        <v>0.3</v>
+        <v>0.4</v>
+      </c>
+      <c r="I17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -916,10 +925,16 @@
         <v>2.4</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="14">
-        <v>0.5</v>
+        <v>0.9</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -929,23 +944,24 @@
       <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="14">
-        <v>0.1</v>
-      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>2.6</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="14"/>
       <c r="I20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1005,7 +1021,7 @@
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="I26" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1033,7 +1049,7 @@
         <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1047,15 +1063,15 @@
         <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
         <v>40</v>
-      </c>
-      <c r="B30" t="s">
-        <v>41</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>10</v>
@@ -1063,10 +1079,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>10</v>
@@ -1074,10 +1090,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>10</v>
@@ -1085,10 +1101,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>10</v>
@@ -1096,10 +1112,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>10</v>
@@ -1107,10 +1123,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>10</v>
@@ -1118,16 +1134,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="s">
         <v>51</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" t="s">
         <v>52</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I36" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1135,7 +1151,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
@@ -1147,7 +1163,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
@@ -1156,30 +1172,30 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E40" s="14">
         <v>0.7</v>
       </c>
       <c r="I40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1187,7 +1203,7 @@
         <v>4.2</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>10</v>
@@ -1198,7 +1214,7 @@
         <v>4.3</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Opstartverslag en fancy diagram
</commit_message>
<xml_diff>
--- a/Planning_Internship_Thesis.xlsx
+++ b/Planning_Internship_Thesis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>Define the deployment Architecture</t>
   </si>
@@ -66,15 +66,6 @@
     <t>Utilize Selenium grid in the execution of web based test suites</t>
   </si>
   <si>
-    <t>1.2.4</t>
-  </si>
-  <si>
-    <t>1.2.5</t>
-  </si>
-  <si>
-    <t>1.2.6</t>
-  </si>
-  <si>
     <t>Utilize Docker container technology in the SDTF runtime</t>
   </si>
   <si>
@@ -100,9 +91,6 @@
   </si>
   <si>
     <t>Create a working demo on the test infrastructure</t>
-  </si>
-  <si>
-    <t>Dependant on 2.1</t>
   </si>
   <si>
     <t>Documentation and thesis</t>
@@ -269,6 +257,15 @@
   </si>
   <si>
     <t>https://askubuntu.com/questions/505506/how-to-get-bash-or-ssh-into-a-running-container-in-background-mode First answer is relevant</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
   </si>
 </sst>
 </file>
@@ -711,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +765,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -777,7 +774,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -788,7 +785,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -797,12 +794,12 @@
         <v>10</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -811,15 +808,15 @@
         <v>0.2</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -840,7 +837,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -851,7 +848,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -863,15 +860,15 @@
         <v>10</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E12" s="14">
         <v>1</v>
@@ -880,7 +877,7 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -888,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -900,7 +897,7 @@
         <v>2.1</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E15" s="14">
         <v>1</v>
@@ -914,13 +911,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E16" s="14">
         <v>0.3</v>
-      </c>
-      <c r="I16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -928,13 +922,13 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E17" s="14">
         <v>0.4</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -942,16 +936,16 @@
         <v>2.4</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E18" s="14">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -959,7 +953,7 @@
         <v>2.5</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>10</v>
@@ -971,14 +965,14 @@
         <v>2.6</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="14"/>
       <c r="I20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -986,7 +980,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -998,7 +992,7 @@
         <v>3.1</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>10</v>
@@ -1009,7 +1003,7 @@
         <v>3.2</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>10</v>
@@ -1020,7 +1014,7 @@
         <v>3.3</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>10</v>
@@ -1031,22 +1025,22 @@
         <v>3.4</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="I26" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>10</v>
@@ -1054,10 +1048,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E28" s="14">
         <v>1</v>
@@ -1066,29 +1060,29 @@
         <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>10</v>
@@ -1096,10 +1090,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>10</v>
@@ -1107,10 +1101,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>10</v>
@@ -1118,10 +1112,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>10</v>
@@ -1129,10 +1123,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>10</v>
@@ -1140,10 +1134,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>10</v>
@@ -1151,16 +1145,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I36" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1168,7 +1162,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
@@ -1180,7 +1174,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
@@ -1189,30 +1183,30 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E40" s="14">
         <v>0.7</v>
       </c>
       <c r="I40" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I41" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1220,7 +1214,7 @@
         <v>4.2</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>10</v>
@@ -1231,7 +1225,7 @@
         <v>4.3</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>10</v>

</xml_diff>